<commit_message>
Slides, Ata e API-Chola
</commit_message>
<xml_diff>
--- a/projeto.sprint_2/TeamDocs/Documentos das Reuniões.xlsx
+++ b/projeto.sprint_2/TeamDocs/Documentos das Reuniões.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Notebook\Desktop\RepositorioRemoto-Sprint2\TeamDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blessed\Desktop\FlowPerAd\projeto.sprint_2\TeamDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47279F57-DB76-41B1-AD96-5DC70B4C8C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25AF052-5635-402A-9954-5BBC3831F1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9E625401-A2BB-4CB0-843B-6F082DD3389E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{9E625401-A2BB-4CB0-843B-6F082DD3389E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Nomes</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Vinicius</t>
   </si>
   <si>
-    <t>Rodrigo</t>
-  </si>
-  <si>
     <t>Matheus</t>
   </si>
   <si>
@@ -95,6 +92,45 @@
   </si>
   <si>
     <t>Tabela de Presença nas Reuniões</t>
+  </si>
+  <si>
+    <t>12º Reunião</t>
+  </si>
+  <si>
+    <t>Soma</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Soma Acumulada</t>
+  </si>
+  <si>
+    <t>Contagem</t>
+  </si>
+  <si>
+    <t>13º Reunião</t>
+  </si>
+  <si>
+    <t>14º Reunião</t>
+  </si>
+  <si>
+    <t>15º Reunião</t>
+  </si>
+  <si>
+    <t>16º Reunião</t>
+  </si>
+  <si>
+    <t>17º Reunião</t>
+  </si>
+  <si>
+    <t>18º Reunião</t>
+  </si>
+  <si>
+    <t>19º Reunião</t>
+  </si>
+  <si>
+    <t>20º Reunião</t>
   </si>
 </sst>
 </file>
@@ -555,65 +591,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA2B6C6-4001-4B00-8619-F692B3F7F2B7}">
-  <dimension ref="B3:N14"/>
+  <dimension ref="B3:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="9.140625" customWidth="1"/>
-    <col min="22" max="28" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="27" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,11 +716,38 @@
       <c r="M4" s="2">
         <v>44673</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>6</v>
+      <c r="N4" s="2">
+        <v>44681</v>
+      </c>
+      <c r="O4" s="2">
+        <v>44688</v>
+      </c>
+      <c r="P4" s="2">
+        <v>44695</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>44702</v>
+      </c>
+      <c r="R4" s="2">
+        <v>44706</v>
+      </c>
+      <c r="S4" s="2">
+        <v>44707</v>
+      </c>
+      <c r="T4" s="2">
+        <v>44708</v>
+      </c>
+      <c r="U4" s="2">
+        <v>44709</v>
+      </c>
+      <c r="V4" s="2">
+        <v>44710</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -671,32 +764,59 @@
         <v>1</v>
       </c>
       <c r="G5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="4">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4">
+        <v>1</v>
+      </c>
+      <c r="P5" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>1</v>
+      </c>
+      <c r="R5" s="4">
+        <v>1</v>
+      </c>
+      <c r="S5" s="4">
+        <v>1</v>
+      </c>
+      <c r="T5" s="4">
+        <v>1</v>
+      </c>
+      <c r="U5" s="4">
+        <v>1</v>
+      </c>
+      <c r="V5" s="4">
+        <v>1</v>
+      </c>
+      <c r="W5" s="4">
         <f>SUM(C5:M5)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -713,32 +833,59 @@
         <v>1</v>
       </c>
       <c r="G6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" ref="N6:N9" si="0">SUM(C6:M6)</f>
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="O6" s="4">
+        <v>1</v>
+      </c>
+      <c r="P6" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>1</v>
+      </c>
+      <c r="R6" s="4">
+        <v>1</v>
+      </c>
+      <c r="S6" s="4">
+        <v>1</v>
+      </c>
+      <c r="T6" s="4">
+        <v>1</v>
+      </c>
+      <c r="U6" s="4">
+        <v>1</v>
+      </c>
+      <c r="V6" s="4">
+        <v>1</v>
+      </c>
+      <c r="W6" s="4">
+        <f>SUM(C6:M6)</f>
+        <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
@@ -755,32 +902,59 @@
         <v>1</v>
       </c>
       <c r="G7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="O7" s="4">
+        <v>1</v>
+      </c>
+      <c r="P7" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>1</v>
+      </c>
+      <c r="R7" s="4">
+        <v>1</v>
+      </c>
+      <c r="S7" s="4">
+        <v>1</v>
+      </c>
+      <c r="T7" s="4">
+        <v>1</v>
+      </c>
+      <c r="U7" s="4">
+        <v>1</v>
+      </c>
+      <c r="V7" s="4">
+        <v>1</v>
+      </c>
+      <c r="W7" s="4">
+        <f>SUM(C7:M7)</f>
+        <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
@@ -797,98 +971,83 @@
         <v>1</v>
       </c>
       <c r="G8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="O8" s="4">
+        <v>1</v>
+      </c>
+      <c r="P8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>1</v>
+      </c>
+      <c r="R8" s="4">
+        <v>1</v>
+      </c>
+      <c r="S8" s="4">
+        <v>1</v>
+      </c>
+      <c r="T8" s="4">
+        <v>1</v>
+      </c>
+      <c r="U8" s="4">
+        <v>1</v>
+      </c>
+      <c r="V8" s="4">
+        <v>1</v>
+      </c>
+      <c r="W8" s="4">
+        <f>SUM(C8:M8)</f>
+        <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4">
-        <v>0</v>
-      </c>
-      <c r="M9" s="4">
-        <v>0</v>
-      </c>
-      <c r="N9" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D10" s="6"/>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F11" s="6"/>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E12" s="6"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H14" s="6"/>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="H13" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B4:B9 C3:N3">
+  <conditionalFormatting sqref="C3:W3 B4:B8">
     <cfRule type="containsText" dxfId="2" priority="10" operator="containsText" text="Nomes">
       <formula>NOT(ISERROR(SEARCH("Nomes",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B9 C3:N3">
+  <conditionalFormatting sqref="C3:W3 B3:B8">
     <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"Tabela de Reuniões"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:N4">
+  <conditionalFormatting sqref="C4:W4">
     <cfRule type="timePeriod" dxfId="0" priority="8" timePeriod="lastMonth">
       <formula>AND(MONTH(C4)=MONTH(EDATE(TODAY(),0-1)),YEAR(C4)=YEAR(EDATE(TODAY(),0-1)))</formula>
     </cfRule>
@@ -905,8 +1064,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:N4 B3">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="B4:W4 B3">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -915,8 +1074,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:N3">
-    <cfRule type="colorScale" priority="18">
+  <conditionalFormatting sqref="C3:W3">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -927,8 +1086,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:N3">
-    <cfRule type="colorScale" priority="20">
+  <conditionalFormatting sqref="C3:W3">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -943,21 +1102,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CD94351161D70F4CAEBD7B86231B3DDF" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5cc1431f9783d4f5e516e1e6dd293d6e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="81d426787a2ad5e2b6fa71d4453f615a" ns3:_="">
     <xsd:import namespace="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29"/>
@@ -1103,31 +1247,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{573AA650-5CBC-49BA-9B70-765C854784D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37428113-CD49-4032-8A81-4D9798B96BD9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A9EC34A-8C12-4FB1-B290-58F74958CD1C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1143,4 +1278,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37428113-CD49-4032-8A81-4D9798B96BD9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{573AA650-5CBC-49BA-9B70-765C854784D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Lógica do leilão atualizada
</commit_message>
<xml_diff>
--- a/projeto.sprint_2/TeamDocs/Documentos das Reuniões.xlsx
+++ b/projeto.sprint_2/TeamDocs/Documentos das Reuniões.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Notebook\Desktop\RepositorioRemoto-Sprint2\TeamDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blessed\Desktop\FlowPerAd\projeto.sprint_2\TeamDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47279F57-DB76-41B1-AD96-5DC70B4C8C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25AF052-5635-402A-9954-5BBC3831F1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9E625401-A2BB-4CB0-843B-6F082DD3389E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{9E625401-A2BB-4CB0-843B-6F082DD3389E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Nomes</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Vinicius</t>
   </si>
   <si>
-    <t>Rodrigo</t>
-  </si>
-  <si>
     <t>Matheus</t>
   </si>
   <si>
@@ -95,6 +92,45 @@
   </si>
   <si>
     <t>Tabela de Presença nas Reuniões</t>
+  </si>
+  <si>
+    <t>12º Reunião</t>
+  </si>
+  <si>
+    <t>Soma</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Soma Acumulada</t>
+  </si>
+  <si>
+    <t>Contagem</t>
+  </si>
+  <si>
+    <t>13º Reunião</t>
+  </si>
+  <si>
+    <t>14º Reunião</t>
+  </si>
+  <si>
+    <t>15º Reunião</t>
+  </si>
+  <si>
+    <t>16º Reunião</t>
+  </si>
+  <si>
+    <t>17º Reunião</t>
+  </si>
+  <si>
+    <t>18º Reunião</t>
+  </si>
+  <si>
+    <t>19º Reunião</t>
+  </si>
+  <si>
+    <t>20º Reunião</t>
   </si>
 </sst>
 </file>
@@ -555,65 +591,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA2B6C6-4001-4B00-8619-F692B3F7F2B7}">
-  <dimension ref="B3:N14"/>
+  <dimension ref="B3:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="9.140625" customWidth="1"/>
-    <col min="22" max="28" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="27" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,11 +716,38 @@
       <c r="M4" s="2">
         <v>44673</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>6</v>
+      <c r="N4" s="2">
+        <v>44681</v>
+      </c>
+      <c r="O4" s="2">
+        <v>44688</v>
+      </c>
+      <c r="P4" s="2">
+        <v>44695</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>44702</v>
+      </c>
+      <c r="R4" s="2">
+        <v>44706</v>
+      </c>
+      <c r="S4" s="2">
+        <v>44707</v>
+      </c>
+      <c r="T4" s="2">
+        <v>44708</v>
+      </c>
+      <c r="U4" s="2">
+        <v>44709</v>
+      </c>
+      <c r="V4" s="2">
+        <v>44710</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -671,32 +764,59 @@
         <v>1</v>
       </c>
       <c r="G5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5" s="4">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4">
+        <v>1</v>
+      </c>
+      <c r="P5" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>1</v>
+      </c>
+      <c r="R5" s="4">
+        <v>1</v>
+      </c>
+      <c r="S5" s="4">
+        <v>1</v>
+      </c>
+      <c r="T5" s="4">
+        <v>1</v>
+      </c>
+      <c r="U5" s="4">
+        <v>1</v>
+      </c>
+      <c r="V5" s="4">
+        <v>1</v>
+      </c>
+      <c r="W5" s="4">
         <f>SUM(C5:M5)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -713,32 +833,59 @@
         <v>1</v>
       </c>
       <c r="G6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" ref="N6:N9" si="0">SUM(C6:M6)</f>
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="O6" s="4">
+        <v>1</v>
+      </c>
+      <c r="P6" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>1</v>
+      </c>
+      <c r="R6" s="4">
+        <v>1</v>
+      </c>
+      <c r="S6" s="4">
+        <v>1</v>
+      </c>
+      <c r="T6" s="4">
+        <v>1</v>
+      </c>
+      <c r="U6" s="4">
+        <v>1</v>
+      </c>
+      <c r="V6" s="4">
+        <v>1</v>
+      </c>
+      <c r="W6" s="4">
+        <f>SUM(C6:M6)</f>
+        <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
@@ -755,32 +902,59 @@
         <v>1</v>
       </c>
       <c r="G7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="O7" s="4">
+        <v>1</v>
+      </c>
+      <c r="P7" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>1</v>
+      </c>
+      <c r="R7" s="4">
+        <v>1</v>
+      </c>
+      <c r="S7" s="4">
+        <v>1</v>
+      </c>
+      <c r="T7" s="4">
+        <v>1</v>
+      </c>
+      <c r="U7" s="4">
+        <v>1</v>
+      </c>
+      <c r="V7" s="4">
+        <v>1</v>
+      </c>
+      <c r="W7" s="4">
+        <f>SUM(C7:M7)</f>
+        <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
@@ -797,98 +971,83 @@
         <v>1</v>
       </c>
       <c r="G8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="O8" s="4">
+        <v>1</v>
+      </c>
+      <c r="P8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>1</v>
+      </c>
+      <c r="R8" s="4">
+        <v>1</v>
+      </c>
+      <c r="S8" s="4">
+        <v>1</v>
+      </c>
+      <c r="T8" s="4">
+        <v>1</v>
+      </c>
+      <c r="U8" s="4">
+        <v>1</v>
+      </c>
+      <c r="V8" s="4">
+        <v>1</v>
+      </c>
+      <c r="W8" s="4">
+        <f>SUM(C8:M8)</f>
+        <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4">
-        <v>0</v>
-      </c>
-      <c r="M9" s="4">
-        <v>0</v>
-      </c>
-      <c r="N9" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D10" s="6"/>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F11" s="6"/>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E12" s="6"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H14" s="6"/>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="H13" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B4:B9 C3:N3">
+  <conditionalFormatting sqref="C3:W3 B4:B8">
     <cfRule type="containsText" dxfId="2" priority="10" operator="containsText" text="Nomes">
       <formula>NOT(ISERROR(SEARCH("Nomes",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B9 C3:N3">
+  <conditionalFormatting sqref="C3:W3 B3:B8">
     <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"Tabela de Reuniões"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:N4">
+  <conditionalFormatting sqref="C4:W4">
     <cfRule type="timePeriod" dxfId="0" priority="8" timePeriod="lastMonth">
       <formula>AND(MONTH(C4)=MONTH(EDATE(TODAY(),0-1)),YEAR(C4)=YEAR(EDATE(TODAY(),0-1)))</formula>
     </cfRule>
@@ -905,8 +1064,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:N4 B3">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="B4:W4 B3">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -915,8 +1074,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:N3">
-    <cfRule type="colorScale" priority="18">
+  <conditionalFormatting sqref="C3:W3">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -927,8 +1086,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:N3">
-    <cfRule type="colorScale" priority="20">
+  <conditionalFormatting sqref="C3:W3">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -943,21 +1102,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CD94351161D70F4CAEBD7B86231B3DDF" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5cc1431f9783d4f5e516e1e6dd293d6e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="81d426787a2ad5e2b6fa71d4453f615a" ns3:_="">
     <xsd:import namespace="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29"/>
@@ -1103,31 +1247,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{573AA650-5CBC-49BA-9B70-765C854784D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37428113-CD49-4032-8A81-4D9798B96BD9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A9EC34A-8C12-4FB1-B290-58F74958CD1C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1143,4 +1278,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37428113-CD49-4032-8A81-4D9798B96BD9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{573AA650-5CBC-49BA-9B70-765C854784D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4bc5c97c-1d73-4ddd-b761-3e2b250dfd29"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>